<commit_message>
Updated individual collection files and updated dates in Billy Paddock collection
</commit_message>
<xml_diff>
--- a/Photographic Archive/PETER HAIN COLLECTION.xlsx
+++ b/Photographic Archive/PETER HAIN COLLECTION.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>identifier</t>
   </si>
@@ -38,6 +38,87 @@
   </si>
   <si>
     <t>file_path</t>
+  </si>
+  <si>
+    <t>ACCESSION NO</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>ACQUISITION NO.</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>ITEM DESCRIPTION</t>
+  </si>
+  <si>
+    <t>LOCATION | SECTION</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t>AR NUMBER</t>
+  </si>
+  <si>
+    <t>2022/23 RFID Number</t>
+  </si>
+  <si>
+    <t>COLLECTIONS</t>
+  </si>
+  <si>
+    <t>EW203-1-1</t>
+  </si>
+  <si>
+    <t>AFRICAN SCHOOL FEEDING SCHEME</t>
+  </si>
+  <si>
+    <t>01/04/2014</t>
+  </si>
+  <si>
+    <t>NEGATIVE B/W MEDIUM FORMAT</t>
+  </si>
+  <si>
+    <t>S-3D (EW 203-208/ EW 210,217/ EW 220,221 &amp; 223) | 3.25</t>
+  </si>
+  <si>
+    <t>421V-PH</t>
+  </si>
+  <si>
+    <t>HAIN, Peter</t>
+  </si>
+  <si>
+    <t>EW204-1-1</t>
+  </si>
+  <si>
+    <t>ANC SCHOOL, GERMEISTON, ANTI BANTU EDUCATION</t>
+  </si>
+  <si>
+    <t>869V-PH</t>
+  </si>
+  <si>
+    <t>EW205-1-1</t>
+  </si>
+  <si>
+    <t>KOAKOA PASS/ APARTHEID PHONE BOOTHS/ SOWETO</t>
+  </si>
+  <si>
+    <t>14370V-PH</t>
+  </si>
+  <si>
+    <t>EW206-1-3</t>
+  </si>
+  <si>
+    <t>HOUSING - CAPE FISHERMEN CA 1936</t>
+  </si>
+  <si>
+    <t>date in title</t>
+  </si>
+  <si>
+    <t>4797V-PH</t>
   </si>
 </sst>
 </file>
@@ -324,7 +405,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -335,6 +416,7 @@
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="39.44140625" customWidth="1"/>
     <col min="8" max="9" width="92.33203125" customWidth="1"/>
+    <col min="11" max="14" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -382,44 +464,152 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="A4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="A6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>

</xml_diff>

<commit_message>
Updated Peter Hain collection
</commit_message>
<xml_diff>
--- a/Photographic Archive/PETER HAIN COLLECTION.xlsx
+++ b/Photographic Archive/PETER HAIN COLLECTION.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>identifier</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>HOUSING - CAPE FISHERMEN CA 1936</t>
-  </si>
-  <si>
-    <t>date in title</t>
   </si>
   <si>
     <t>4797V-PH</t>
@@ -405,7 +402,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -589,8 +586,8 @@
       <c r="C6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>33</v>
+      <c r="D6" s="5">
+        <v>1936</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>11</v>
@@ -605,7 +602,7 @@
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N6" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Removed acquisition date from from Peter Hain collection
</commit_message>
<xml_diff>
--- a/Photographic Archive/PETER HAIN COLLECTION.xlsx
+++ b/Photographic Archive/PETER HAIN COLLECTION.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>identifier</t>
   </si>
@@ -40,24 +40,9 @@
     <t>file_path</t>
   </si>
   <si>
-    <t>ACCESSION NO</t>
-  </si>
-  <si>
-    <t>TITLE</t>
-  </si>
-  <si>
-    <t>ACQUISITION NO.</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
-    <t>ITEM DESCRIPTION</t>
-  </si>
-  <si>
-    <t>LOCATION | SECTION</t>
-  </si>
-  <si>
     <t>QTY</t>
   </si>
   <si>
@@ -74,9 +59,6 @@
   </si>
   <si>
     <t>AFRICAN SCHOOL FEEDING SCHEME</t>
-  </si>
-  <si>
-    <t>01/04/2014</t>
   </si>
   <si>
     <t>NEGATIVE B/W MEDIUM FORMAT</t>
@@ -398,11 +380,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z68"/>
+  <dimension ref="A1:Z67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -412,8 +394,9 @@
     <col min="5" max="5" width="15.109375" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="39.44140625" customWidth="1"/>
-    <col min="8" max="9" width="92.33203125" customWidth="1"/>
-    <col min="11" max="14" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" customWidth="1"/>
+    <col min="11" max="14" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -443,11 +426,19 @@
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -462,151 +453,121 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="D3" s="5"/>
       <c r="E3" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D4" s="5"/>
       <c r="E4" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1936</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1936</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" t="s">
-        <v>24</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -768,7 +729,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="C27" s="4"/>
       <c r="D27" s="5"/>
@@ -1096,14 +1057,6 @@
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
     </row>
-    <row r="68" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="3"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated collection data in Peter Hain collection
</commit_message>
<xml_diff>
--- a/Photographic Archive/PETER HAIN COLLECTION.xlsx
+++ b/Photographic Archive/PETER HAIN COLLECTION.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -382,9 +382,9 @@
   </sheetPr>
   <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>